<commit_message>
Backlog de requisitos atualizado
</commit_message>
<xml_diff>
--- a/documentos/arquivos/Backlog Requisitos.xlsx
+++ b/documentos/arquivos/Backlog Requisitos.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/bruno_lima_sptech_school/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/henrique_coelho_sptech_school/Documents/SPTECH/GIT/VagaFacil/documentos/arquivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3109E303-F01C-42E0-89C2-F88A6112C560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{3109E303-F01C-42E0-89C2-F88A6112C560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37BC9EF1-4A54-422C-9052-58178F4FDD0B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9332CED2-CA08-4B4F-8188-CC5E418AAD90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +24,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="181">
   <si>
     <t>Vaga Fácil</t>
   </si>
@@ -529,6 +525,57 @@
   </si>
   <si>
     <t>Criar um diagrama de visão de negócio sobre os nossos serviços ao cliente</t>
+  </si>
+  <si>
+    <t>Fluxograma de atendimento de suporte</t>
+  </si>
+  <si>
+    <t>Fluxograma representando o processo realizado durante o atendimento ao cliente</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Tabelas criadas no AZURE</t>
+  </si>
+  <si>
+    <t>Script do banco de dados criando as tabelas na nuvem AZURE</t>
+  </si>
+  <si>
+    <t>Configuração e integração do JIRA</t>
+  </si>
+  <si>
+    <t>Configurar a nossa ferramenta de Help Desk de acordo com o projeto e a regra de negócio</t>
+  </si>
+  <si>
+    <t>Integração do site com a nuvem</t>
+  </si>
+  <si>
+    <t>Subir todos os arquivos referentes ao nosso site na nuvem AZURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual de instalação </t>
+  </si>
+  <si>
+    <t>Manual organizado e intuitivo mostrando para o usuário o passo a passo para a instalação do produto, desde a parte física até a explicação do dashboard</t>
+  </si>
+  <si>
+    <t>Selecionar os dados do banco e mostrá-los nos nossos gráficos exibindo os alertas de acordo com as nossas métricas</t>
+  </si>
+  <si>
+    <t>Teste integrado do Analytics</t>
+  </si>
+  <si>
+    <t>Teste integrado da solução de IoT</t>
+  </si>
+  <si>
+    <t>Capturar os dados do arduíno, salvar no banco, selecionar esses dados e integrá-los aos nossos gráficos e kpi´s</t>
+  </si>
+  <si>
+    <t>Cadastro, Login e Dashboard conectados com BD na nuvem</t>
+  </si>
+  <si>
+    <t>Sessão de dashboard funcional, conectados com o banco de dados na nuvem AZURE</t>
   </si>
 </sst>
 </file>
@@ -602,7 +649,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -769,11 +816,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -850,6 +927,55 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2341,34 +2467,34 @@
       <selection activeCell="B36" sqref="B36:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.7109375" customWidth="1"/>
-    <col min="3" max="3" width="60.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="60.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="22"/>
       <c r="C3" s="23"/>
       <c r="D3" s="24"/>
     </row>
-    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -2380,7 +2506,7 @@
       </c>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2391,7 +2517,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2402,7 +2528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -2413,7 +2539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2424,7 +2550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2435,7 +2561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
@@ -2446,14 +2572,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2464,7 +2590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
@@ -2475,7 +2601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2486,7 +2612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -2497,7 +2623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
@@ -2508,7 +2634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
@@ -2519,7 +2645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>31</v>
       </c>
@@ -2530,7 +2656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
@@ -2541,7 +2667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>35</v>
       </c>
@@ -2552,7 +2678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
@@ -2563,14 +2689,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
@@ -2581,7 +2707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
@@ -2592,7 +2718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>44</v>
       </c>
@@ -2603,14 +2729,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
@@ -2621,7 +2747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
@@ -2632,7 +2758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>52</v>
       </c>
@@ -2643,7 +2769,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>54</v>
       </c>
@@ -2654,7 +2780,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>54</v>
       </c>
@@ -2665,7 +2791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>57</v>
       </c>
@@ -2676,7 +2802,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>60</v>
       </c>
@@ -2687,7 +2813,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>62</v>
       </c>
@@ -2698,7 +2824,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
         <v>64</v>
       </c>
@@ -2724,48 +2850,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A16856E6-9DCD-40AD-91F7-EC610FDB522F}">
-  <dimension ref="A2:O56"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="29"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="H3" s="30"/>
+    </row>
+    <row r="4" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="26"/>
@@ -2773,10 +2900,10 @@
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-    </row>
-    <row r="5" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:15" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2794,13 +2921,13 @@
       <c r="G5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="35" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -2818,7 +2945,7 @@
       <c r="G6" s="10">
         <v>9</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="36">
         <v>2</v>
       </c>
       <c r="J6" s="15" t="s">
@@ -2840,9 +2967,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="37" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -2860,7 +2987,7 @@
       <c r="G7" s="11">
         <v>2</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="38">
         <v>1</v>
       </c>
       <c r="J7" s="11">
@@ -2883,9 +3010,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="35" t="s">
         <v>115</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2903,13 +3030,13 @@
       <c r="G8" s="10">
         <v>18</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="37" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="11" t="s">
@@ -2927,7 +3054,7 @@
       <c r="G9" s="11">
         <v>19</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="38">
         <v>2</v>
       </c>
       <c r="J9" s="15" t="s">
@@ -2949,9 +3076,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="35" t="s">
         <v>127</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -2969,7 +3096,7 @@
       <c r="G10" s="10">
         <v>3</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="36">
         <v>1</v>
       </c>
       <c r="J10" s="11">
@@ -2997,9 +3124,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="37" t="s">
         <v>128</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -3017,14 +3144,14 @@
       <c r="G11" s="11">
         <v>4</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="38">
         <v>1</v>
       </c>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="35" t="s">
         <v>162</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -3042,13 +3169,13 @@
       <c r="G12" s="10">
         <v>28</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="37" t="s">
         <v>160</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -3066,13 +3193,13 @@
       <c r="G13" s="11">
         <v>26</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="35" t="s">
         <v>149</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -3090,13 +3217,13 @@
       <c r="G14" s="10">
         <v>39</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="37" t="s">
         <v>86</v>
       </c>
       <c r="C15" s="11" t="s">
@@ -3114,13 +3241,13 @@
       <c r="G15" s="11">
         <v>27</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="35" t="s">
         <v>150</v>
       </c>
       <c r="C16" s="10"/>
@@ -3136,13 +3263,13 @@
       <c r="G16" s="10">
         <v>40</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="37" t="s">
         <v>131</v>
       </c>
       <c r="C17" s="11" t="s">
@@ -3160,13 +3287,13 @@
       <c r="G17" s="11">
         <v>31</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="35" t="s">
         <v>152</v>
       </c>
       <c r="C18" s="10"/>
@@ -3182,13 +3309,13 @@
       <c r="G18" s="10">
         <v>42</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="37" t="s">
         <v>129</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -3206,13 +3333,13 @@
       <c r="G19" s="11">
         <v>35</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="35" t="s">
         <v>106</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -3230,13 +3357,13 @@
       <c r="G20" s="10">
         <v>11</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="37" t="s">
         <v>132</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -3254,13 +3381,13 @@
       <c r="G21" s="11">
         <v>32</v>
       </c>
-      <c r="H21" s="11">
+      <c r="H21" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="35" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -3278,13 +3405,13 @@
       <c r="G22" s="10">
         <v>5</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="37" t="s">
         <v>116</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -3302,14 +3429,14 @@
       <c r="G23" s="11">
         <v>10</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="38">
         <v>2</v>
       </c>
       <c r="J23" s="13"/>
     </row>
-    <row r="24" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="35" t="s">
         <v>117</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -3327,13 +3454,13 @@
       <c r="G24" s="10">
         <v>12</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="37" t="s">
         <v>93</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -3351,13 +3478,13 @@
       <c r="G25" s="11">
         <v>17</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="35" t="s">
         <v>130</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -3375,13 +3502,13 @@
       <c r="G26" s="10">
         <v>33</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="37" t="s">
         <v>143</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -3399,13 +3526,13 @@
       <c r="G27" s="11">
         <v>21</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H27" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="35" t="s">
         <v>134</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -3423,13 +3550,13 @@
       <c r="G28" s="10">
         <v>36</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="37" t="s">
         <v>142</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -3447,13 +3574,13 @@
       <c r="G29" s="11">
         <v>22</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="35" t="s">
         <v>133</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -3471,13 +3598,13 @@
       <c r="G30" s="10">
         <v>34</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="37" t="s">
         <v>118</v>
       </c>
       <c r="C31" s="11" t="s">
@@ -3495,13 +3622,13 @@
       <c r="G31" s="11">
         <v>7</v>
       </c>
-      <c r="H31" s="11">
+      <c r="H31" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="35" t="s">
         <v>80</v>
       </c>
       <c r="C32" s="10" t="s">
@@ -3519,13 +3646,13 @@
       <c r="G32" s="10">
         <v>6</v>
       </c>
-      <c r="H32" s="10">
+      <c r="H32" s="36">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="37" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="11" t="s">
@@ -3543,13 +3670,13 @@
       <c r="G33" s="11">
         <v>1</v>
       </c>
-      <c r="H33" s="11">
+      <c r="H33" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="35" t="s">
         <v>79</v>
       </c>
       <c r="C34" s="10" t="s">
@@ -3567,13 +3694,13 @@
       <c r="G34" s="10">
         <v>25</v>
       </c>
-      <c r="H34" s="10">
+      <c r="H34" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="37" t="s">
         <v>120</v>
       </c>
       <c r="C35" s="11" t="s">
@@ -3591,13 +3718,13 @@
       <c r="G35" s="11">
         <v>8</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="35" t="s">
         <v>121</v>
       </c>
       <c r="C36" s="10" t="s">
@@ -3615,13 +3742,13 @@
       <c r="G36" s="10">
         <v>37</v>
       </c>
-      <c r="H36" s="10">
+      <c r="H36" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="37" t="s">
         <v>122</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -3639,13 +3766,13 @@
       <c r="G37" s="11">
         <v>38</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H37" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="35" t="s">
         <v>109</v>
       </c>
       <c r="C38" s="10" t="s">
@@ -3663,13 +3790,13 @@
       <c r="G38" s="10">
         <v>13</v>
       </c>
-      <c r="H38" s="10">
+      <c r="H38" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="37" t="s">
         <v>90</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -3687,13 +3814,13 @@
       <c r="G39" s="11">
         <v>16</v>
       </c>
-      <c r="H39" s="11">
+      <c r="H39" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="35" t="s">
         <v>100</v>
       </c>
       <c r="C40" s="10" t="s">
@@ -3711,13 +3838,13 @@
       <c r="G40" s="10">
         <v>14</v>
       </c>
-      <c r="H40" s="10">
+      <c r="H40" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="37" t="s">
         <v>151</v>
       </c>
       <c r="C41" s="11"/>
@@ -3733,13 +3860,13 @@
       <c r="G41" s="11">
         <v>41</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="35" t="s">
         <v>126</v>
       </c>
       <c r="C42" s="10" t="s">
@@ -3757,13 +3884,13 @@
       <c r="G42" s="10">
         <v>24</v>
       </c>
-      <c r="H42" s="10">
+      <c r="H42" s="36">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="37" t="s">
         <v>125</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -3781,13 +3908,13 @@
       <c r="G43" s="11">
         <v>20</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="35" t="s">
         <v>119</v>
       </c>
       <c r="C44" s="10" t="s">
@@ -3805,13 +3932,13 @@
       <c r="G44" s="10">
         <v>23</v>
       </c>
-      <c r="H44" s="10">
+      <c r="H44" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="37" t="s">
         <v>153</v>
       </c>
       <c r="C45" s="11"/>
@@ -3827,13 +3954,13 @@
       <c r="G45" s="11">
         <v>43</v>
       </c>
-      <c r="H45" s="11">
+      <c r="H45" s="38">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="35" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="10" t="s">
@@ -3851,13 +3978,13 @@
       <c r="G46" s="10">
         <v>30</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H46" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="37" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="11" t="s">
@@ -3875,40 +4002,179 @@
       <c r="G47" s="11">
         <v>24</v>
       </c>
-      <c r="H47" s="11">
+      <c r="H47" s="38">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-    </row>
-    <row r="54" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-    </row>
-    <row r="55" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-    </row>
-    <row r="56" spans="2:8" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="10">
+        <v>5</v>
+      </c>
+      <c r="G48" s="10"/>
+      <c r="H48" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B49" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="F49" s="27">
+        <v>5</v>
+      </c>
+      <c r="G49" s="28"/>
+      <c r="H49" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B50" s="35" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F50" s="10">
+        <v>8</v>
+      </c>
+      <c r="G50" s="10"/>
+      <c r="H50" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B51" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F51" s="27">
+        <v>8</v>
+      </c>
+      <c r="G51" s="28"/>
+      <c r="H51" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="10">
+        <v>13</v>
+      </c>
+      <c r="G52" s="10"/>
+      <c r="H52" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="11">
+        <v>13</v>
+      </c>
+      <c r="G53" s="11"/>
+      <c r="H53" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="10">
+        <v>13</v>
+      </c>
+      <c r="G54" s="10"/>
+      <c r="H54" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E55" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="F55" s="41">
+        <v>21</v>
+      </c>
+      <c r="G55" s="41"/>
+      <c r="H55" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
@@ -3929,6 +4195,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d029c515-0698-44b3-a257-13b9aeaa6222" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100304D1BD6A797FA429AD32DD54426A246" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e35a718f99b259fb6f4d5b2085aee5ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d029c515-0698-44b3-a257-13b9aeaa6222" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2e3a67cfaa2d42426d64ed184a490dd0" ns3:_="">
     <xsd:import namespace="d029c515-0698-44b3-a257-13b9aeaa6222"/>
@@ -4110,24 +4393,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23153AD-BE05-4DA6-A5C3-260C487D4A4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="d029c515-0698-44b3-a257-13b9aeaa6222"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d029c515-0698-44b3-a257-13b9aeaa6222" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59D1CCA-49A8-465E-BB52-99854B7FF734}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02990EA6-9E1D-4811-AE24-4FA311A213B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4143,28 +4433,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C59D1CCA-49A8-465E-BB52-99854B7FF734}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D23153AD-BE05-4DA6-A5C3-260C487D4A4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="d029c515-0698-44b3-a257-13b9aeaa6222"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>